<commit_message>
remove error from rentBikeTransaction
</commit_message>
<xml_diff>
--- a/Requirements Analysis/UseCaseSpecification.xlsx
+++ b/Requirements Analysis/UseCaseSpecification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftwareDesignAndConstruction\TKXDPM.KSTN.20201-08\Requirements Analysis\Use case specification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftwareDesignAndConstruction\TKXDPM.KSTN.20201-08\Requirements Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C725B63F-C629-4390-9B3D-00314DD9520F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26D4021-B5A6-414C-A115-4878C07492AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11835" tabRatio="597" activeTab="2" xr2:uid="{9E918315-6A42-422F-903B-03B968EF713D}"/>
+    <workbookView xWindow="12330" yWindow="-120" windowWidth="21600" windowHeight="11835" tabRatio="597" activeTab="3" xr2:uid="{9E918315-6A42-422F-903B-03B968EF713D}"/>
   </bookViews>
   <sheets>
     <sheet name="viewBikeInDock" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="119">
   <si>
     <t>Luồng sự kiện chính</t>
   </si>
@@ -503,16 +503,10 @@
     <t>Danh sách bãi xe</t>
   </si>
   <si>
-    <t>Khoảng cách</t>
-  </si>
-  <si>
     <t>Số 1, Đại Cồ Việt</t>
   </si>
   <si>
     <t>Bãi xe Bách khoa</t>
-  </si>
-  <si>
-    <t>Đơn vị (m)</t>
   </si>
   <si>
     <t>Chỉ dành cho xe
@@ -582,9 +576,6 @@
   </si>
   <si>
     <t>Là số nguyên dương</t>
-  </si>
-  <si>
-    <t>Số nguyên dương</t>
   </si>
   <si>
     <t>Hiển thị giao dịch trả xe và thông báo thành công</t>
@@ -856,7 +847,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -931,8 +922,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -952,18 +952,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1003,22 +991,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1030,6 +1009,18 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1040,22 +1031,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1393,54 +1381,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
@@ -1449,12 +1437,12 @@
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2">
@@ -1463,12 +1451,12 @@
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="C7" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2">
@@ -1477,52 +1465,52 @@
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="11" t="s">
@@ -1537,10 +1525,10 @@
       <c r="D13" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="28"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="7">
@@ -1553,10 +1541,10 @@
       <c r="D14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="32">
         <v>20173284442</v>
       </c>
-      <c r="F14" s="29"/>
+      <c r="F14" s="32"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="7">
@@ -1569,26 +1557,26 @@
       <c r="D15" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="29"/>
+      <c r="F15" s="32"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" customHeight="1">
       <c r="A16" s="7">
         <v>3</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="33">
         <v>4000000</v>
       </c>
-      <c r="F16" s="29"/>
+      <c r="F16" s="32"/>
     </row>
     <row r="17" spans="1:6" ht="30">
       <c r="A17" s="7">
@@ -1598,11 +1586,11 @@
         <v>33</v>
       </c>
       <c r="C17" s="7"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="30">
+      <c r="D17" s="34"/>
+      <c r="E17" s="33">
         <v>10000</v>
       </c>
-      <c r="F17" s="29"/>
+      <c r="F17" s="32"/>
     </row>
     <row r="18" spans="1:6" ht="45" customHeight="1">
       <c r="A18" s="7">
@@ -1612,11 +1600,11 @@
         <v>35</v>
       </c>
       <c r="C18" s="7"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="30">
+      <c r="D18" s="34"/>
+      <c r="E18" s="33">
         <v>3000</v>
       </c>
-      <c r="F18" s="29"/>
+      <c r="F18" s="32"/>
     </row>
     <row r="19" spans="1:6" ht="30">
       <c r="A19" s="7">
@@ -1631,10 +1619,10 @@
       <c r="D19" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="32">
         <v>60</v>
       </c>
-      <c r="F19" s="29"/>
+      <c r="F19" s="32"/>
     </row>
     <row r="20" spans="1:6" ht="30">
       <c r="A20" s="7">
@@ -1649,10 +1637,10 @@
       <c r="D20" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="35">
         <v>3.5</v>
       </c>
-      <c r="F20" s="32"/>
+      <c r="F20" s="35"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="7">
@@ -1665,23 +1653,34 @@
       <c r="D21" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="29"/>
+      <c r="F21" s="32"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="A12:F12"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A10:F10"/>
@@ -1694,17 +1693,6 @@
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1735,54 +1723,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="A1" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="19" t="s">
@@ -1791,12 +1779,12 @@
       <c r="B6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="18">
@@ -1805,12 +1793,12 @@
       <c r="B7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="C7" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="18">
@@ -1819,52 +1807,52 @@
       <c r="B8" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="C8" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="20" t="s">
@@ -1879,10 +1867,10 @@
       <c r="D13" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="28"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="17">
@@ -1895,50 +1883,50 @@
       <c r="D14" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="29"/>
+      <c r="F14" s="32"/>
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1">
       <c r="A15" s="17">
         <v>2</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" s="30">
+        <v>88</v>
+      </c>
+      <c r="E15" s="33">
         <v>400000</v>
       </c>
-      <c r="F15" s="29"/>
+      <c r="F15" s="32"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="39">
+      <c r="A16" s="38">
         <v>3</v>
       </c>
-      <c r="B16" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="37" t="s">
+      <c r="B16" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="38"/>
+      <c r="D16" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="42">
         <v>60000</v>
       </c>
-      <c r="F16" s="44"/>
+      <c r="F16" s="43"/>
     </row>
     <row r="17" spans="1:6" ht="45" customHeight="1">
-      <c r="A17" s="40"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="46"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="45"/>
     </row>
     <row r="18" spans="1:6" ht="30">
       <c r="A18" s="17">
@@ -1953,30 +1941,29 @@
       <c r="D18" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="32">
         <v>60</v>
       </c>
-      <c r="F18" s="29"/>
+      <c r="F18" s="32"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E15:F15"/>
@@ -1986,12 +1973,13 @@
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="A12:F12"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="E16:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2002,7 +1990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD398524-161E-4778-AD6A-3ED7F5DE324A}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
@@ -2024,54 +2012,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="9" t="s">
@@ -2080,12 +2068,12 @@
       <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="8">
@@ -2094,12 +2082,12 @@
       <c r="B7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="8">
@@ -2108,12 +2096,12 @@
       <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="8">
@@ -2122,12 +2110,12 @@
       <c r="B9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="8">
@@ -2136,12 +2124,12 @@
       <c r="B10" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="7">
@@ -2150,12 +2138,12 @@
       <c r="B11" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="49"/>
+      <c r="C11" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="48"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="24">
@@ -2164,12 +2152,12 @@
       <c r="B12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" spans="1:6" ht="30">
       <c r="A13" s="24">
@@ -2178,12 +2166,12 @@
       <c r="B13" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="7">
@@ -2192,12 +2180,12 @@
       <c r="B14" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
+      <c r="C14" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="17">
@@ -2206,12 +2194,12 @@
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
+      <c r="C15" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="10">
@@ -2220,12 +2208,12 @@
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="49"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="48"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="24">
@@ -2234,12 +2222,12 @@
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="49"/>
+      <c r="C17" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="48"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="10">
@@ -2248,12 +2236,12 @@
       <c r="B18" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="10">
@@ -2262,12 +2250,12 @@
       <c r="B19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="51" t="s">
+      <c r="C19" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="10">
@@ -2276,12 +2264,12 @@
       <c r="B20" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="51" t="s">
+      <c r="C20" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="6">
@@ -2290,12 +2278,12 @@
       <c r="B21" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="51" t="s">
+      <c r="C21" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="10">
@@ -2318,12 +2306,12 @@
       <c r="B23" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="51" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
+      <c r="C23" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1">
@@ -2333,21 +2321,21 @@
         <v>5</v>
       </c>
       <c r="C24" s="60" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D24" s="61"/>
       <c r="E24" s="61"/>
       <c r="F24" s="62"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="52" t="s">
+      <c r="A25" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="52"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="9" t="s">
@@ -2380,10 +2368,10 @@
       <c r="D27" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="51" t="s">
+      <c r="E27" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="F27" s="51"/>
+      <c r="F27" s="49"/>
     </row>
     <row r="28" spans="1:6" ht="30">
       <c r="A28" s="10">
@@ -2398,10 +2386,10 @@
       <c r="D28" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E28" s="50">
+      <c r="E28" s="55">
         <v>2</v>
       </c>
-      <c r="F28" s="50"/>
+      <c r="F28" s="55"/>
     </row>
     <row r="29" spans="1:6" ht="30">
       <c r="A29" s="10">
@@ -2416,40 +2404,40 @@
       <c r="D29" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E29" s="50" t="s">
+      <c r="E29" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="F29" s="51"/>
+      <c r="F29" s="49"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="55"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="58"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="13" t="s">
@@ -2464,10 +2452,10 @@
       <c r="D33" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E33" s="28" t="s">
+      <c r="E33" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F33" s="28"/>
+      <c r="F33" s="31"/>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1">
       <c r="A34" s="12">
@@ -2480,10 +2468,10 @@
       <c r="D34" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E34" s="29" t="s">
+      <c r="E34" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F34" s="29"/>
+      <c r="F34" s="32"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="12">
@@ -2493,13 +2481,13 @@
         <v>34</v>
       </c>
       <c r="C35" s="12"/>
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="30">
+      <c r="E35" s="33">
         <v>400000</v>
       </c>
-      <c r="F35" s="29"/>
+      <c r="F35" s="32"/>
     </row>
     <row r="36" spans="1:6" ht="30">
       <c r="A36" s="12">
@@ -2509,11 +2497,11 @@
         <v>33</v>
       </c>
       <c r="C36" s="12"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="30">
+      <c r="D36" s="34"/>
+      <c r="E36" s="33">
         <v>10000</v>
       </c>
-      <c r="F36" s="29"/>
+      <c r="F36" s="32"/>
     </row>
     <row r="37" spans="1:6" ht="60">
       <c r="A37" s="12">
@@ -2523,11 +2511,11 @@
         <v>35</v>
       </c>
       <c r="C37" s="12"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="30">
+      <c r="D37" s="34"/>
+      <c r="E37" s="33">
         <v>3000</v>
       </c>
-      <c r="F37" s="29"/>
+      <c r="F37" s="32"/>
     </row>
     <row r="38" spans="1:6" ht="45">
       <c r="A38" s="12">
@@ -2537,15 +2525,15 @@
         <v>36</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="29">
+      <c r="E38" s="32">
         <v>60</v>
       </c>
-      <c r="F38" s="29"/>
+      <c r="F38" s="32"/>
     </row>
     <row r="39" spans="1:6" ht="30">
       <c r="A39" s="12">
@@ -2555,15 +2543,15 @@
         <v>40</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E39" s="32">
+      <c r="E39" s="35">
         <v>3.5</v>
       </c>
-      <c r="F39" s="32"/>
+      <c r="F39" s="35"/>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="12">
@@ -2576,20 +2564,20 @@
       <c r="D40" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E40" s="29" t="s">
+      <c r="E40" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="F40" s="29"/>
+      <c r="F40" s="32"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A41" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
+      <c r="A41" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="20" t="s">
@@ -2604,10 +2592,10 @@
       <c r="D42" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E42" s="28" t="s">
+      <c r="E42" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F42" s="28"/>
+      <c r="F42" s="31"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="17">
@@ -2618,28 +2606,28 @@
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E43" s="29">
+        <v>96</v>
+      </c>
+      <c r="E43" s="32">
         <v>1213124123</v>
       </c>
-      <c r="F43" s="29"/>
+      <c r="F43" s="32"/>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="23">
         <v>2</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C44" s="23"/>
       <c r="D44" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="E44" s="29">
+        <v>96</v>
+      </c>
+      <c r="E44" s="32">
         <v>101012345</v>
       </c>
-      <c r="F44" s="29"/>
+      <c r="F44" s="32"/>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="23">
@@ -2652,121 +2640,157 @@
       <c r="D45" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E45" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="F45" s="29"/>
+      <c r="E45" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="F45" s="32"/>
     </row>
     <row r="46" spans="1:6" ht="30">
       <c r="A46" s="23">
         <v>4</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C46" s="23"/>
       <c r="D46" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="E46" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="F46" s="29"/>
+        <v>103</v>
+      </c>
+      <c r="E46" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F46" s="32"/>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="23">
         <v>5</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="E47" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="F47" s="29"/>
+        <v>103</v>
+      </c>
+      <c r="E47" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="F47" s="32"/>
     </row>
     <row r="48" spans="1:6" ht="30">
       <c r="A48" s="23">
         <v>6</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C48" s="23"/>
       <c r="D48" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="E48" s="30">
+        <v>96</v>
+      </c>
+      <c r="E48" s="33">
         <v>100000</v>
       </c>
-      <c r="F48" s="29"/>
+      <c r="F48" s="32"/>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="23">
         <v>7</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C49" s="23"/>
       <c r="D49" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E49" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="F49" s="30"/>
+      <c r="E49" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="F49" s="33"/>
     </row>
     <row r="50" spans="1:6" ht="30">
       <c r="A50" s="23">
         <v>8</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C50" s="23"/>
       <c r="D50" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="E50" s="30">
+        <v>96</v>
+      </c>
+      <c r="E50" s="33">
         <v>100000</v>
       </c>
-      <c r="F50" s="30"/>
+      <c r="F50" s="33"/>
     </row>
     <row r="51" spans="1:6" ht="45">
       <c r="A51" s="23">
         <v>9</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C51" s="23"/>
       <c r="D51" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="E51" s="30">
+        <v>96</v>
+      </c>
+      <c r="E51" s="33">
         <v>20000</v>
       </c>
-      <c r="F51" s="30"/>
+      <c r="F51" s="33"/>
     </row>
     <row r="52" spans="1:6" ht="30" customHeight="1">
-      <c r="A52" s="56" t="s">
-        <v>114</v>
-      </c>
-      <c r="B52" s="57"/>
-      <c r="C52" s="57"/>
-      <c r="D52" s="57"/>
-      <c r="E52" s="57"/>
-      <c r="F52" s="58"/>
+      <c r="A52" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="B52" s="53"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C17:F17"/>
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="C10:F10"/>
@@ -2783,42 +2807,6 @@
     <mergeCell ref="A25:F25"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E37:F37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2827,10 +2815,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B92BA79D-BD45-431B-810E-32D40CF25167}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2851,54 +2839,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="9" t="s">
@@ -2907,12 +2895,12 @@
       <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="8">
@@ -2921,12 +2909,12 @@
       <c r="B7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="8">
@@ -2935,12 +2923,12 @@
       <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="8">
@@ -2949,12 +2937,12 @@
       <c r="B9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="8">
@@ -2963,12 +2951,12 @@
       <c r="B10" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="8">
@@ -2977,12 +2965,12 @@
       <c r="B11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="24">
@@ -2992,7 +2980,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="60" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D12" s="61"/>
       <c r="E12" s="61"/>
@@ -3006,7 +2994,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="60" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D13" s="61"/>
       <c r="E13" s="61"/>
@@ -3019,12 +3007,12 @@
       <c r="B14" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="51" t="s">
+      <c r="C14" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="7">
@@ -3033,12 +3021,12 @@
       <c r="B15" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="7">
@@ -3047,12 +3035,12 @@
       <c r="B16" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1">
       <c r="A17" s="10">
@@ -3061,12 +3049,12 @@
       <c r="B17" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="65" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
+      <c r="C17" s="66" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="14">
@@ -3076,21 +3064,21 @@
         <v>5</v>
       </c>
       <c r="C18" s="60" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D18" s="61"/>
       <c r="E18" s="61"/>
       <c r="F18" s="62"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="9" t="s">
@@ -3123,40 +3111,40 @@
       <c r="D21" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="51" t="s">
+      <c r="E21" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="F21" s="51"/>
+      <c r="F21" s="49"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="52" t="s">
+      <c r="A22" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="67" t="s">
+      <c r="A24" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="11" t="s">
@@ -3171,10 +3159,10 @@
       <c r="D25" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="28" t="s">
+      <c r="E25" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="28"/>
+      <c r="F25" s="31"/>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1">
       <c r="A26" s="7">
@@ -3187,10 +3175,10 @@
       <c r="D26" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" s="64"/>
+      <c r="E26" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="F26" s="63"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="7">
@@ -3203,20 +3191,20 @@
       <c r="D27" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="64" t="s">
-        <v>80</v>
-      </c>
-      <c r="F27" s="64"/>
+      <c r="E27" s="63" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" s="63"/>
     </row>
     <row r="28" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A28" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
+      <c r="A28" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="22" t="s">
@@ -3231,10 +3219,10 @@
       <c r="D29" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="E29" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F29" s="28"/>
+      <c r="F29" s="31"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="23">
@@ -3245,28 +3233,28 @@
       </c>
       <c r="C30" s="23"/>
       <c r="D30" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="E30" s="29">
+        <v>96</v>
+      </c>
+      <c r="E30" s="32">
         <v>1213124123</v>
       </c>
-      <c r="F30" s="29"/>
+      <c r="F30" s="32"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="23">
         <v>2</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C31" s="23"/>
       <c r="D31" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="E31" s="29">
+        <v>96</v>
+      </c>
+      <c r="E31" s="32">
         <v>101012345</v>
       </c>
-      <c r="F31" s="29"/>
+      <c r="F31" s="32"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="23">
@@ -3279,154 +3267,145 @@
       <c r="D32" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="F32" s="29"/>
+      <c r="E32" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" s="32"/>
     </row>
     <row r="33" spans="1:6" ht="30">
       <c r="A33" s="23">
         <v>4</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C33" s="23"/>
       <c r="D33" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="F33" s="29"/>
+        <v>103</v>
+      </c>
+      <c r="E33" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F33" s="32"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="23">
         <v>5</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="E34" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="F34" s="29"/>
+        <v>103</v>
+      </c>
+      <c r="E34" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34" s="32"/>
     </row>
     <row r="35" spans="1:6" ht="30">
       <c r="A35" s="23">
         <v>6</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C35" s="23"/>
       <c r="D35" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="E35" s="30">
+        <v>96</v>
+      </c>
+      <c r="E35" s="33">
         <v>100000</v>
       </c>
-      <c r="F35" s="29"/>
+      <c r="F35" s="32"/>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="23">
         <v>7</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C36" s="23"/>
       <c r="D36" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="F36" s="30"/>
+      <c r="E36" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="F36" s="33"/>
     </row>
     <row r="37" spans="1:6" ht="30">
       <c r="A37" s="23">
         <v>8</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C37" s="23"/>
       <c r="D37" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="E37" s="30">
+        <v>96</v>
+      </c>
+      <c r="E37" s="33">
         <v>100000</v>
       </c>
-      <c r="F37" s="30"/>
+      <c r="F37" s="33"/>
     </row>
     <row r="38" spans="1:6" ht="45">
       <c r="A38" s="23">
         <v>9</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C38" s="23"/>
       <c r="D38" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="E38" s="30">
+        <v>96</v>
+      </c>
+      <c r="E38" s="33">
         <v>20000</v>
       </c>
-      <c r="F38" s="30"/>
+      <c r="F38" s="33"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="7">
-        <v>6</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="E39" s="64">
-        <v>600</v>
-      </c>
-      <c r="F39" s="64"/>
+      <c r="A39" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="66" t="s">
-        <v>119</v>
-      </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="27"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="A40:F41"/>
+  <mergeCells count="38">
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="A39:F40"/>
     <mergeCell ref="A22:F22"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="A24:F24"/>
@@ -3438,27 +3417,17 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="E38:F38"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Requirement Analysis: Return bike and view Bike
</commit_message>
<xml_diff>
--- a/Requirements Analysis/UseCaseSpecification.xlsx
+++ b/Requirements Analysis/UseCaseSpecification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftwareDesignAndConstruction\TKXDPM.KSTN.20201-08\Requirements Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26D4021-B5A6-414C-A115-4878C07492AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3067E1-C651-472F-90B5-E6E27462BF79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12330" yWindow="-120" windowWidth="21600" windowHeight="11835" tabRatio="597" activeTab="3" xr2:uid="{9E918315-6A42-422F-903B-03B968EF713D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="597" xr2:uid="{9E918315-6A42-422F-903B-03B968EF713D}"/>
   </bookViews>
   <sheets>
     <sheet name="viewBikeInDock" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="129">
   <si>
     <t>Luồng sự kiện chính</t>
   </si>
@@ -246,9 +246,6 @@
     <t>Mã vạch</t>
   </si>
   <si>
-    <t>Số nguyên</t>
-  </si>
-  <si>
     <t>Loại xe</t>
   </si>
   <si>
@@ -506,9 +503,6 @@
     <t>Số 1, Đại Cồ Việt</t>
   </si>
   <si>
-    <t>Bãi xe Bách khoa</t>
-  </si>
-  <si>
     <t>Chỉ dành cho xe
 điện</t>
   </si>
@@ -581,9 +575,6 @@
     <t>Hiển thị giao dịch trả xe và thông báo thành công</t>
   </si>
   <si>
-    <t>Giá xe</t>
-  </si>
-  <si>
     <t>Lấy thông tin thẻ của người dùng</t>
   </si>
   <si>
@@ -606,12 +597,6 @@
     <t>Thời gian trả</t>
   </si>
   <si>
-    <t>Sau khi trả xe</t>
-  </si>
-  <si>
-    <t>9:00 am, 20/11/2020</t>
-  </si>
-  <si>
     <t>Chi phí thuê xe</t>
   </si>
   <si>
@@ -633,18 +618,64 @@
     <t>Giá thuê 15 phút sau 30 phút đầu</t>
   </si>
   <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Luôn là NULL</t>
+  </si>
+  <si>
     <t>Cập nhật và lưu lại giao dịch thuê xe, giao dịch trừ tiền,
-cập nhật trạng thái xe, bãi xe</t>
-  </si>
-  <si>
-    <t>Hậu điều kiện: Thay đổi trạng thái của xe thành không sử dụng, hoàn thành giao dịch thanh toán 
-và trả tiền cọc cho người dùng, cập nhật và lưu lại giao dịch thuê xe</t>
-  </si>
-  <si>
-    <t>NULL</t>
-  </si>
-  <si>
-    <t>Luôn là NULL</t>
+cập nhật trạng thái xe và địa chỉ bãi xe mới tương ứng</t>
+  </si>
+  <si>
+    <t>Đại học Bách khoa Hà nội</t>
+  </si>
+  <si>
+    <t>202000012020-12-15 10:58:25</t>
+  </si>
+  <si>
+    <t>Xe đạp điện</t>
+  </si>
+  <si>
+    <t>Vũ Trung Nghĩa</t>
+  </si>
+  <si>
+    <t>Giá thuê 30 phút đầu</t>
+  </si>
+  <si>
+    <t>Thời điểm thuê xe</t>
+  </si>
+  <si>
+    <t>2020-12-15 10:58:29</t>
+  </si>
+  <si>
+    <t>Thời điểm trả xe</t>
+  </si>
+  <si>
+    <t>2020-12-15 10:59:36</t>
+  </si>
+  <si>
+    <t>Tiền đặt cọc</t>
+  </si>
+  <si>
+    <t>Số nguyên dương</t>
+  </si>
+  <si>
+    <t>Hậu điều kiện: Thay đổi trạng thái của xe thành không sử dụng và cập nhật lại địa chị bãi xe mới của xe hóa đơn thuê xe được cập nhật và lưu lại, giao dịch trả tiền được lưu lại</t>
+  </si>
+  <si>
+    <t>Giá trị</t>
+  </si>
+  <si>
+    <t>Lượng pin còn
+lại (%)</t>
+  </si>
+  <si>
+    <t>Là số thực</t>
+  </si>
+  <si>
+    <t>Thời gian sử 
+dụng tối đa (h)</t>
   </si>
 </sst>
 </file>
@@ -847,7 +878,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -922,16 +953,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -952,6 +974,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -982,22 +1016,34 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1009,41 +1055,44 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1361,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51002064-996C-4651-AF61-0FB299FD3525}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1381,54 +1430,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
@@ -1437,12 +1486,12 @@
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2">
@@ -1451,12 +1500,12 @@
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
+      <c r="C7" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2">
@@ -1465,52 +1514,52 @@
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
+      <c r="A12" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="11" t="s">
@@ -1525,10 +1574,10 @@
       <c r="D13" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="31"/>
+      <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="7">
@@ -1539,148 +1588,137 @@
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="32">
-        <v>20173284442</v>
-      </c>
-      <c r="F14" s="32"/>
+        <v>123</v>
+      </c>
+      <c r="E14" s="29">
+        <v>20200017</v>
+      </c>
+      <c r="F14" s="29"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="7">
         <v>2</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="32"/>
+        <v>30</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" s="29"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" customHeight="1">
       <c r="A16" s="7">
         <v>3</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="33">
-        <v>4000000</v>
-      </c>
-      <c r="F16" s="32"/>
+      <c r="D16" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="30">
+        <v>1200000</v>
+      </c>
+      <c r="F16" s="29"/>
     </row>
     <row r="17" spans="1:6" ht="30">
       <c r="A17" s="7">
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="7"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="33">
-        <v>10000</v>
-      </c>
-      <c r="F17" s="32"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="30">
+        <v>15000</v>
+      </c>
+      <c r="F17" s="29"/>
     </row>
     <row r="18" spans="1:6" ht="45" customHeight="1">
       <c r="A18" s="7">
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="7"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="33">
-        <v>3000</v>
-      </c>
-      <c r="F18" s="32"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="30">
+        <v>5000</v>
+      </c>
+      <c r="F18" s="29"/>
     </row>
     <row r="19" spans="1:6" ht="30">
       <c r="A19" s="7">
         <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>36</v>
+        <v>126</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="32">
-        <v>60</v>
-      </c>
-      <c r="F19" s="32"/>
+        <v>37</v>
+      </c>
+      <c r="E19" s="29">
+        <v>100</v>
+      </c>
+      <c r="F19" s="29"/>
     </row>
     <row r="20" spans="1:6" ht="30">
       <c r="A20" s="7">
         <v>7</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="35">
+        <v>127</v>
+      </c>
+      <c r="E20" s="32">
         <v>3.5</v>
       </c>
-      <c r="F20" s="35"/>
+      <c r="F20" s="32"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="7">
         <v>8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="32"/>
+        <v>30</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="29"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
     <mergeCell ref="A12:F12"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A10:F10"/>
@@ -1693,6 +1731,17 @@
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1723,54 +1772,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="A1" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="A4" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="19" t="s">
@@ -1779,12 +1828,12 @@
       <c r="B6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="18">
@@ -1793,12 +1842,12 @@
       <c r="B7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
+      <c r="C7" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="18">
@@ -1807,52 +1856,52 @@
       <c r="B8" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="C8" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
+      <c r="A12" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="20" t="s">
@@ -1867,103 +1916,104 @@
       <c r="D13" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="31"/>
+      <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="17">
         <v>1</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="32"/>
+      <c r="F14" s="29"/>
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1">
       <c r="A15" s="17">
         <v>2</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="33">
+        <v>86</v>
+      </c>
+      <c r="E15" s="30">
         <v>400000</v>
       </c>
-      <c r="F15" s="32"/>
+      <c r="F15" s="29"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="38">
+      <c r="A16" s="39">
         <v>3</v>
       </c>
-      <c r="B16" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="42">
+      <c r="B16" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="43">
         <v>60000</v>
       </c>
-      <c r="F16" s="43"/>
+      <c r="F16" s="44"/>
     </row>
     <row r="17" spans="1:6" ht="45" customHeight="1">
-      <c r="A17" s="39"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="45"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="46"/>
     </row>
     <row r="18" spans="1:6" ht="30">
       <c r="A18" s="17">
         <v>6</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="32">
+        <v>37</v>
+      </c>
+      <c r="E18" s="29">
         <v>60</v>
       </c>
-      <c r="F18" s="32"/>
+      <c r="F18" s="29"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="E16:F17"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E15:F15"/>
@@ -1973,13 +2023,12 @@
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="A12:F12"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2012,54 +2061,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
+      <c r="A3" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="9" t="s">
@@ -2068,12 +2117,12 @@
       <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="8">
@@ -2082,12 +2131,12 @@
       <c r="B7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="49" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
+      <c r="C7" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="8">
@@ -2096,12 +2145,12 @@
       <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
+      <c r="C8" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="8">
@@ -2110,12 +2159,12 @@
       <c r="B9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
+      <c r="C9" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="8">
@@ -2124,12 +2173,12 @@
       <c r="B10" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
+      <c r="C10" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="7">
@@ -2138,12 +2187,12 @@
       <c r="B11" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="48"/>
+      <c r="C11" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="62"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="24">
@@ -2152,26 +2201,26 @@
       <c r="B12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
+      <c r="C12" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
     </row>
     <row r="13" spans="1:6" ht="30">
       <c r="A13" s="24">
         <v>7</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
+        <v>45</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="7">
@@ -2180,12 +2229,12 @@
       <c r="B14" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
+      <c r="C14" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="17">
@@ -2194,12 +2243,12 @@
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
+      <c r="C15" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="10">
@@ -2208,12 +2257,12 @@
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="48"/>
+      <c r="C16" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="62"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="24">
@@ -2222,12 +2271,12 @@
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="48"/>
+      <c r="C17" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="62"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="10">
@@ -2236,12 +2285,12 @@
       <c r="B18" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
+      <c r="C18" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="10">
@@ -2250,12 +2299,12 @@
       <c r="B19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
+      <c r="C19" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="10">
@@ -2264,12 +2313,12 @@
       <c r="B20" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
+      <c r="C20" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="6">
@@ -2278,12 +2327,12 @@
       <c r="B21" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
+      <c r="C21" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="10">
@@ -2292,12 +2341,12 @@
       <c r="B22" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="59"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59"/>
+      <c r="C22" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="21">
@@ -2306,12 +2355,12 @@
       <c r="B23" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="49" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
+      <c r="C23" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1">
@@ -2320,22 +2369,22 @@
       <c r="B24" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="62"/>
+      <c r="C24" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="51"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="9" t="s">
@@ -2363,15 +2412,15 @@
         <v>10</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="F27" s="49"/>
+      <c r="F27" s="47"/>
     </row>
     <row r="28" spans="1:6" ht="30">
       <c r="A28" s="10">
@@ -2381,15 +2430,15 @@
         <v>6</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" s="55">
+        <v>61</v>
+      </c>
+      <c r="E28" s="52">
         <v>2</v>
       </c>
-      <c r="F28" s="55"/>
+      <c r="F28" s="52"/>
     </row>
     <row r="29" spans="1:6" ht="30">
       <c r="A29" s="10">
@@ -2402,42 +2451,42 @@
         <v>11</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E29" s="55" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29" s="49"/>
+        <v>63</v>
+      </c>
+      <c r="E29" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="47"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="58"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="56"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="50" t="s">
+      <c r="A31" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1">
-      <c r="A32" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
+      <c r="A32" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="13" t="s">
@@ -2452,132 +2501,132 @@
       <c r="D33" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E33" s="31" t="s">
+      <c r="E33" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F33" s="31"/>
+      <c r="F33" s="28"/>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1">
       <c r="A34" s="12">
         <v>1</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E34" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="F34" s="32"/>
+      <c r="F34" s="29"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="12">
         <v>2</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35" s="12"/>
-      <c r="D35" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="E35" s="33">
+      <c r="D35" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="30">
         <v>400000</v>
       </c>
-      <c r="F35" s="32"/>
+      <c r="F35" s="29"/>
     </row>
     <row r="36" spans="1:6" ht="30">
       <c r="A36" s="12">
         <v>3</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C36" s="12"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="33">
+      <c r="D36" s="31"/>
+      <c r="E36" s="30">
         <v>10000</v>
       </c>
-      <c r="F36" s="32"/>
+      <c r="F36" s="29"/>
     </row>
     <row r="37" spans="1:6" ht="60">
       <c r="A37" s="12">
         <v>4</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" s="12"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="33">
+      <c r="D37" s="31"/>
+      <c r="E37" s="30">
         <v>3000</v>
       </c>
-      <c r="F37" s="32"/>
+      <c r="F37" s="29"/>
     </row>
     <row r="38" spans="1:6" ht="45">
       <c r="A38" s="12">
         <v>5</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" s="32">
+        <v>37</v>
+      </c>
+      <c r="E38" s="29">
         <v>60</v>
       </c>
-      <c r="F38" s="32"/>
+      <c r="F38" s="29"/>
     </row>
     <row r="39" spans="1:6" ht="30">
       <c r="A39" s="12">
         <v>6</v>
       </c>
       <c r="B39" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E39" s="35">
+      <c r="E39" s="32">
         <v>3.5</v>
       </c>
-      <c r="F39" s="35"/>
+      <c r="F39" s="32"/>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="12">
         <v>7</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E40" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="F40" s="32"/>
+        <v>30</v>
+      </c>
+      <c r="E40" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" s="29"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A41" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
+      <c r="A41" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="20" t="s">
@@ -2592,10 +2641,10 @@
       <c r="D42" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E42" s="31" t="s">
+      <c r="E42" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F42" s="31"/>
+      <c r="F42" s="28"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="17">
@@ -2606,168 +2655,178 @@
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="E43" s="32">
+        <v>94</v>
+      </c>
+      <c r="E43" s="29">
         <v>1213124123</v>
       </c>
-      <c r="F43" s="32"/>
+      <c r="F43" s="29"/>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="23">
         <v>2</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C44" s="23"/>
       <c r="D44" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E44" s="32">
+        <v>94</v>
+      </c>
+      <c r="E44" s="29">
         <v>101012345</v>
       </c>
-      <c r="F44" s="32"/>
+      <c r="F44" s="29"/>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="23">
         <v>3</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C45" s="23"/>
       <c r="D45" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E45" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="F45" s="32"/>
+        <v>30</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" s="29"/>
     </row>
     <row r="46" spans="1:6" ht="30">
       <c r="A46" s="23">
         <v>4</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C46" s="23"/>
       <c r="D46" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="E46" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="F46" s="32"/>
+        <v>100</v>
+      </c>
+      <c r="E46" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="F46" s="29"/>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="23">
         <v>5</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="E47" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="F47" s="32"/>
+        <v>100</v>
+      </c>
+      <c r="E47" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="F47" s="29"/>
     </row>
     <row r="48" spans="1:6" ht="30">
       <c r="A48" s="23">
         <v>6</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C48" s="23"/>
       <c r="D48" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E48" s="33">
+        <v>94</v>
+      </c>
+      <c r="E48" s="30">
         <v>100000</v>
       </c>
-      <c r="F48" s="32"/>
+      <c r="F48" s="29"/>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="23">
         <v>7</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C49" s="23"/>
       <c r="D49" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E49" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="F49" s="33"/>
+        <v>30</v>
+      </c>
+      <c r="E49" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F49" s="30"/>
     </row>
     <row r="50" spans="1:6" ht="30">
       <c r="A50" s="23">
         <v>8</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C50" s="23"/>
       <c r="D50" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E50" s="33">
+        <v>94</v>
+      </c>
+      <c r="E50" s="30">
         <v>100000</v>
       </c>
-      <c r="F50" s="33"/>
+      <c r="F50" s="30"/>
     </row>
     <row r="51" spans="1:6" ht="45">
       <c r="A51" s="23">
         <v>9</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C51" s="23"/>
       <c r="D51" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E51" s="33">
+        <v>94</v>
+      </c>
+      <c r="E51" s="30">
         <v>20000</v>
       </c>
-      <c r="F51" s="33"/>
+      <c r="F51" s="30"/>
     </row>
     <row r="52" spans="1:6" ht="30" customHeight="1">
-      <c r="A52" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="B52" s="53"/>
-      <c r="C52" s="53"/>
-      <c r="D52" s="53"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="54"/>
+      <c r="A52" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="B52" s="58"/>
+      <c r="C52" s="58"/>
+      <c r="D52" s="58"/>
+      <c r="E52" s="58"/>
+      <c r="F52" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C17:F17"/>
     <mergeCell ref="A52:F52"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E38:F38"/>
@@ -2784,29 +2843,19 @@
     <mergeCell ref="D35:D37"/>
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="E46:F46"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C23:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2815,10 +2864,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B92BA79D-BD45-431B-810E-32D40CF25167}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2826,9 +2875,9 @@
     <col min="1" max="1" width="6.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="19.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="32.5703125" style="1" customWidth="1"/>
@@ -2839,54 +2888,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="49" t="s">
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="9" t="s">
@@ -2895,12 +2944,12 @@
       <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="8">
@@ -2909,12 +2958,12 @@
       <c r="B7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
+      <c r="C7" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="8">
@@ -2923,12 +2972,12 @@
       <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
+      <c r="C8" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="8">
@@ -2937,12 +2986,12 @@
       <c r="B9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
+      <c r="C9" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="8">
@@ -2951,12 +3000,12 @@
       <c r="B10" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
+      <c r="C10" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="8">
@@ -2965,12 +3014,12 @@
       <c r="B11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
+      <c r="C11" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="24">
@@ -2979,12 +3028,12 @@
       <c r="B12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="62"/>
+      <c r="C12" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="51"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="24">
@@ -2993,12 +3042,12 @@
       <c r="B13" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="60" t="s">
-        <v>99</v>
-      </c>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="62"/>
+      <c r="C13" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="51"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="24">
@@ -3007,12 +3056,12 @@
       <c r="B14" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
+      <c r="C14" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="7">
@@ -3021,12 +3070,12 @@
       <c r="B15" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
+      <c r="C15" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="7">
@@ -3035,12 +3084,12 @@
       <c r="B16" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
+      <c r="C16" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1">
       <c r="A17" s="10">
@@ -3049,12 +3098,12 @@
       <c r="B17" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="66" t="s">
-        <v>115</v>
-      </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
+      <c r="C17" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="14">
@@ -3063,22 +3112,22 @@
       <c r="B18" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="62"/>
+      <c r="C18" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="51"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="9" t="s">
@@ -3106,45 +3155,45 @@
         <v>5</v>
       </c>
       <c r="C21" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="47"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="53"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" s="49"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="50"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="65" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="11" t="s">
@@ -3159,10 +3208,10 @@
       <c r="D25" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="31"/>
+      <c r="F25" s="28"/>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1">
       <c r="A26" s="7">
@@ -3173,12 +3222,12 @@
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" s="63" t="s">
-        <v>80</v>
-      </c>
-      <c r="F26" s="63"/>
+        <v>30</v>
+      </c>
+      <c r="E26" s="67" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="67"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="7">
@@ -3189,22 +3238,22 @@
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" s="63" t="s">
-        <v>79</v>
-      </c>
-      <c r="F27" s="63"/>
+        <v>30</v>
+      </c>
+      <c r="E27" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="F27" s="67"/>
     </row>
     <row r="28" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A28" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
+      <c r="A28" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="22" t="s">
@@ -3219,10 +3268,10 @@
       <c r="D29" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F29" s="31"/>
+      <c r="F29" s="28"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="23">
@@ -3233,96 +3282,94 @@
       </c>
       <c r="C30" s="23"/>
       <c r="D30" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="E30" s="32">
+        <v>94</v>
+      </c>
+      <c r="E30" s="29">
         <v>1213124123</v>
       </c>
-      <c r="F30" s="32"/>
+      <c r="F30" s="29"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="23">
         <v>2</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C31" s="23"/>
       <c r="D31" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E31" s="32">
-        <v>101012345</v>
-      </c>
-      <c r="F31" s="32"/>
+        <v>30</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="F31" s="29"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="23">
         <v>3</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" s="23"/>
       <c r="D32" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="F32" s="32"/>
+        <v>30</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="29"/>
     </row>
     <row r="33" spans="1:6" ht="30">
       <c r="A33" s="23">
         <v>4</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C33" s="23"/>
       <c r="D33" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="E33" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="F33" s="32"/>
+        <v>94</v>
+      </c>
+      <c r="E33" s="30">
+        <v>25000</v>
+      </c>
+      <c r="F33" s="29"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="23">
         <v>5</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" s="23" t="s">
-        <v>106</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="C34" s="23"/>
       <c r="D34" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="E34" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="F34" s="32"/>
+        <v>30</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="F34" s="29"/>
     </row>
     <row r="35" spans="1:6" ht="30">
       <c r="A35" s="23">
         <v>6</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="C35" s="23"/>
       <c r="D35" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E35" s="33">
-        <v>100000</v>
-      </c>
-      <c r="F35" s="32"/>
-    </row>
-    <row r="36" spans="1:6">
+        <v>94</v>
+      </c>
+      <c r="E35" s="70">
+        <v>15000</v>
+      </c>
+      <c r="F35" s="71"/>
+    </row>
+    <row r="36" spans="1:6" ht="45">
       <c r="A36" s="23">
         <v>7</v>
       </c>
@@ -3331,81 +3378,92 @@
       </c>
       <c r="C36" s="23"/>
       <c r="D36" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E36" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="F36" s="33"/>
+        <v>94</v>
+      </c>
+      <c r="E36" s="70">
+        <v>5000</v>
+      </c>
+      <c r="F36" s="70"/>
     </row>
     <row r="37" spans="1:6" ht="30">
-      <c r="A37" s="23">
+      <c r="A37" s="26">
         <v>8</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C37" s="23"/>
+        <v>118</v>
+      </c>
+      <c r="C37" s="26"/>
       <c r="D37" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E37" s="33">
-        <v>100000</v>
-      </c>
-      <c r="F37" s="33"/>
-    </row>
-    <row r="38" spans="1:6" ht="45">
-      <c r="A38" s="23">
+        <v>30</v>
+      </c>
+      <c r="E37" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="F37" s="69"/>
+    </row>
+    <row r="38" spans="1:6" ht="30">
+      <c r="A38" s="26">
         <v>9</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C38" s="23"/>
+        <v>120</v>
+      </c>
+      <c r="C38" s="26"/>
       <c r="D38" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E38" s="33">
-        <v>20000</v>
-      </c>
-      <c r="F38" s="33"/>
+        <v>30</v>
+      </c>
+      <c r="E38" s="68" t="s">
+        <v>121</v>
+      </c>
+      <c r="F38" s="69"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
+      <c r="A39" s="26">
+        <v>10</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" s="26"/>
+      <c r="D39" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="E39" s="72">
+        <v>480000</v>
+      </c>
+      <c r="F39" s="69"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="30"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
+      <c r="A40" s="65" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="A39:F40"/>
+  <mergeCells count="39">
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="A40:F41"/>
     <mergeCell ref="A22:F22"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="A24:F24"/>
@@ -3418,16 +3476,22 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
     <mergeCell ref="A28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>